<commit_message>
[REQ]21143 - Add producer code to excel
</commit_message>
<xml_diff>
--- a/clients/ArrowHead/data/template/DOC_and_UM_CarPort_Design.xlsx
+++ b/clients/ArrowHead/data/template/DOC_and_UM_CarPort_Design.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Producer Code – producerCode</t>
+  </si>
   <si>
     <t xml:space="preserve">Drive Other Car &amp; Higher UM/UIM Limits/Deductibles</t>
   </si>
@@ -89,7 +92,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -111,12 +114,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,16 +165,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -202,10 +195,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:N18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -218,84 +211,89 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.43"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
         <v>19</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>